<commit_message>
calculate and add current KPI
</commit_message>
<xml_diff>
--- a/Equip_F/Results/KPIs.xlsx
+++ b/Equip_F/Results/KPIs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,30 @@
         <v>96.34</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Madrid</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>918.97</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>checkin</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>96.22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add dashboard in tableau
</commit_message>
<xml_diff>
--- a/Equip_F/Results/KPIs.xlsx
+++ b/Equip_F/Results/KPIs.xlsx
@@ -1,37 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liubovshubina/Documents/IT/Projects/25_Simulator/ProjecteData/Equip_F/Results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>1_OccupancyRate</t>
+  </si>
+  <si>
+    <t>2_HighestOccupancy</t>
+  </si>
+  <si>
+    <t>3_Satisfaction Index</t>
+  </si>
+  <si>
+    <t>4_HighestSatisfactionItem</t>
+  </si>
+  <si>
+    <t>4_Score</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Check-in</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,24 +91,34 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -133,6 +188,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,120 +480,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sprint</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>1_OccupancyRate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2_HighestOccupancy</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>3_Satisfaction Index</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>4_HighestSatisfactionItem</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>4_Score</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>59.03</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Madrid</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>919.99</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Communication</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>96.43000000000001</v>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>96.43</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>58.65</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Madrid</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>919.3099999999999</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Communication</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>919.31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
         <v>96.34</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>56.5</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Madrid</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>918.97</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Check-in</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
         <v>96.22</v>
       </c>
     </row>

</xml_diff>